<commit_message>
update Work plan.xlsx and README.md
</commit_message>
<xml_diff>
--- a/docs/Work plan.xlsx
+++ b/docs/Work plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vista\Documents\semester 8\Photonic Device\Self-learning-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vista\Documents\semester 8\Photonic Device\Self-learning-project\photonic_device\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2397950-F259-408C-863A-CF3E5CFEBC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFB9C80-9734-4527-9B6A-A3E3ED267E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -104,7 +104,37 @@
     <t>Longitudinal phase modulator</t>
   </si>
   <si>
-    <t>Lithium Niobate medium</t>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>1 h</t>
+  </si>
+  <si>
+    <t>No need to be random</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lithium Niobate medium 
+Release v1.0.0
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <t>29/09/21</t>
   </si>
 </sst>
 </file>
@@ -196,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -212,15 +242,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -229,13 +250,31 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,6 +312,164 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1590675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="412934" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE07EE9-C039-4D66-AA0C-34A0D7782AA2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9772650" y="1166812"/>
+              <a:ext cx="412934" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐿𝑖𝑁</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑂</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>3</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BE07EE9-C039-4D66-AA0C-34A0D7782AA2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9772650" y="1166812"/>
+              <a:ext cx="412934" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐿𝑖𝑁𝑂_3</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,7 +738,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,111 +789,129 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="11">
-        <v>1</v>
-      </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="E2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="16" t="s">
+      <c r="E3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="14" t="s">
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="14" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="11" t="s">
+    <row r="5" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="18"/>
+      <c r="C5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="14" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="14" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -716,6 +931,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>

<commit_message>
initial commit for amplitude modulator
</commit_message>
<xml_diff>
--- a/docs/Work plan.xlsx
+++ b/docs/Work plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vista\Documents\semester 8\Photonic Device\Self-learning-project\photonic_device\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A85E99E-C71C-44DE-AA77-382C1A837EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B59E727-6B03-4B4E-BC7F-BFFBFCE2D6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -140,15 +140,25 @@
     <t>Optical Polarization Modulator</t>
   </si>
   <si>
+    <t>30/09/21</t>
+  </si>
+  <si>
+    <t>Transverse polarization modulator</t>
+  </si>
+  <si>
+    <t>Optical Amplitude Modulator</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lithium Niobate medium 
-Release v1.0.0
+Release v2.0.0
 </t>
   </si>
   <si>
-    <t>30/09/21</t>
-  </si>
-  <si>
-    <t>Transverse polarization modulator</t>
+    <t>GaAs polarization modulator
+Release v3.0.0</t>
+  </si>
+  <si>
+    <t>Longitudinal polarization modulator</t>
   </si>
 </sst>
 </file>
@@ -240,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -273,6 +283,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -284,23 +312,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,8 +516,8 @@
       <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="412934" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -592,7 +605,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -915,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,31 +950,31 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="18" t="s">
         <v>9</v>
       </c>
     </row>
@@ -969,7 +982,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -998,7 +1011,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
@@ -1025,7 +1038,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -1052,7 +1065,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="13" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1090,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="18"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="6" t="s">
         <v>23</v>
       </c>
@@ -1099,22 +1112,51 @@
       <c r="B7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="19" t="s">
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="9" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1124,7 +1166,7 @@
     <mergeCell ref="B4:B6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
@@ -1142,13 +1184,13 @@
           <x14:formula1>
             <xm:f>Variables!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I7</xm:sqref>
+          <xm:sqref>I2:I8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50E2DA23-DD80-49FE-B624-FDE87E63F771}">
           <x14:formula1>
             <xm:f>Variables!$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J7</xm:sqref>
+          <xm:sqref>J2:J8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>